<commit_message>
My Tasks products Approval Updated
</commit_message>
<xml_diff>
--- a/src/assets/samples/DispatchedToDelivered.xlsx
+++ b/src/assets/samples/DispatchedToDelivered.xlsx
@@ -37,9 +37,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -67,12 +67,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -130,12 +124,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -143,11 +145,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -231,28 +233,29 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" s="4" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+    <row r="2" s="6" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="n">
+      <c r="B2" s="5" t="n">
         <v>367</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes in Excel Date Format
</commit_message>
<xml_diff>
--- a/src/assets/samples/DispatchedToDelivered.xlsx
+++ b/src/assets/samples/DispatchedToDelivered.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">PurchaseOrderNumber</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t xml:space="preserve">LR-TL-1-10000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31-12-2018</t>
   </si>
 </sst>
 </file>
@@ -233,7 +236,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -255,8 +258,8 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="n">
-        <v>367</v>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>